<commit_message>
ppu pin asignment updated.
</commit_message>
<xml_diff>
--- a/doc/super-duper-nes-hardware-design.xlsx
+++ b/doc/super-duper-nes-hardware-design.xlsx
@@ -198,9 +198,6 @@
     <t>28:CHR-D2</t>
   </si>
   <si>
-    <t>58:CHR-A6</t>
-  </si>
-  <si>
     <t>29:CHR-D3</t>
   </si>
   <si>
@@ -333,6 +330,10 @@
   </si>
   <si>
     <t>基板厚は1.2mm</t>
+  </si>
+  <si>
+    <t>58:CHR-D6</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -1231,7 +1232,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1275,7 +1276,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1295,7 +1296,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1330,7 +1331,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1350,7 +1351,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1618,7 +1619,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1638,7 +1639,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1673,7 +1674,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1693,7 +1694,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -5542,7 +5543,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5560,33 +5561,33 @@
   <sheetData>
     <row r="11" spans="28:60">
       <c r="AL11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>66</v>
       </c>
-      <c r="AQ11" t="s">
-        <v>67</v>
-      </c>
       <c r="BH11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="28:60">
       <c r="AX13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="28:60">
       <c r="AB15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="33:33">
       <c r="AG24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="33:33">
       <c r="AG25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -5602,7 +5603,7 @@
   <dimension ref="B2:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5625,7 +5626,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="14.25" thickBot="1">
@@ -5636,7 +5637,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.25" thickBot="1">
@@ -5647,7 +5648,7 @@
         <v>6</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="14.25" thickBot="1">
@@ -5658,7 +5659,7 @@
         <v>8</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="14.25" thickBot="1">
@@ -5669,7 +5670,7 @@
         <v>10</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="14.25" thickBot="1">
@@ -5680,7 +5681,7 @@
         <v>12</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="14.25" thickBot="1">
@@ -5691,7 +5692,7 @@
         <v>14</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="14.25" thickBot="1">
@@ -5702,7 +5703,7 @@
         <v>16</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="14.25" thickBot="1">
@@ -5870,23 +5871,23 @@
         <v>57</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="14.25" thickBot="1">
       <c r="B32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="14.25" thickBot="1">
       <c r="B33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -5919,7 +5920,7 @@
   <sheetData>
     <row r="3" spans="5:18">
       <c r="J3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="5:18">
@@ -5927,10 +5928,10 @@
         <v>1</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P6" s="6">
         <v>2</v>
@@ -5941,10 +5942,10 @@
         <v>3</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P8" s="6">
         <v>4</v>
@@ -5955,10 +5956,10 @@
         <v>5</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P10" s="6">
         <v>6</v>
@@ -5969,10 +5970,10 @@
         <v>7</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P12" s="6">
         <v>8</v>
@@ -5983,10 +5984,10 @@
         <v>9</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P14" s="6">
         <v>10</v>
@@ -5994,22 +5995,22 @@
     </row>
     <row r="16" spans="5:18">
       <c r="E16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H16" s="6">
         <v>11</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P16" s="6">
         <v>12</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="8:16">
@@ -6017,10 +6018,10 @@
         <v>13</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P18" s="6">
         <v>14</v>
@@ -6031,10 +6032,10 @@
         <v>15</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P20" s="6">
         <v>16</v>
@@ -6045,10 +6046,10 @@
         <v>17</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P22" s="6">
         <v>18</v>
@@ -6059,10 +6060,10 @@
         <v>19</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P24" s="6">
         <v>20</v>
@@ -6073,10 +6074,10 @@
         <v>21</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P26" s="6">
         <v>22</v>
@@ -6087,10 +6088,10 @@
         <v>23</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P28" s="6">
         <v>24</v>
@@ -6101,10 +6102,10 @@
         <v>25</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P30" s="6">
         <v>26</v>
@@ -6115,10 +6116,10 @@
         <v>27</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P32" s="6">
         <v>28</v>
@@ -6126,22 +6127,22 @@
     </row>
     <row r="34" spans="5:18">
       <c r="E34" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H34" s="6">
         <v>29</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P34" s="6">
         <v>30</v>
       </c>
       <c r="R34" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="5:18">
@@ -6149,10 +6150,10 @@
         <v>31</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P36" s="6">
         <v>32</v>
@@ -6163,10 +6164,10 @@
         <v>33</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P38" s="6">
         <v>34</v>
@@ -6177,10 +6178,10 @@
         <v>35</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P40" s="6">
         <v>36</v>
@@ -6191,10 +6192,10 @@
         <v>37</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P42" s="6">
         <v>38</v>
@@ -6205,10 +6206,10 @@
         <v>39</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P44" s="6">
         <v>40</v>
@@ -6248,32 +6249,32 @@
   <sheetData>
     <row r="3" spans="2:10">
       <c r="B3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="15">
         <v>-0.3</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="15">
         <v>-0.3</v>
@@ -6282,14 +6283,14 @@
     <row r="6" spans="2:10">
       <c r="B6" s="15"/>
       <c r="C6" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="16">
         <v>0.4</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H6" s="15">
         <v>0.8</v>
@@ -6297,19 +6298,19 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="16">
         <v>2.4</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="15">
         <v>1.7</v>
@@ -6318,14 +6319,14 @@
     <row r="8" spans="2:10">
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8" s="16">
         <v>5</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H8" s="15">
         <v>3.6</v>
@@ -6333,19 +6334,19 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="16">
         <v>0.8</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="15">
         <v>0.8</v>
@@ -6354,14 +6355,14 @@
     <row r="10" spans="2:10">
       <c r="B10" s="15"/>
       <c r="C10" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="16">
         <v>2</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H10" s="15">
         <v>1.7</v>
@@ -6369,35 +6370,35 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="15">
         <v>0.4</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" s="14">
         <v>0.2</v>
@@ -6405,19 +6406,19 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="15">
         <v>2.4</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H13" s="14">
         <v>3.1</v>
@@ -6426,17 +6427,17 @@
     <row r="14" spans="2:10">
       <c r="B14" s="15"/>
       <c r="C14" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:10">
@@ -6449,7 +6450,7 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="12"/>
@@ -6457,15 +6458,15 @@
       <c r="G16" s="13"/>
       <c r="H16" s="12"/>
       <c r="J16" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -6521,7 +6522,7 @@
         <v>3.8</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I24" s="8">
         <v>3.8</v>
@@ -6559,7 +6560,7 @@
         <v>3</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -6599,7 +6600,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I33" s="8">
         <v>2</v>
@@ -6658,7 +6659,7 @@
         <v>0.6</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I40" s="8">
         <v>0.6</v>
@@ -6686,13 +6687,13 @@
         <v>0</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I43" s="8">
         <v>0</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -6713,10 +6714,10 @@
     </row>
     <row r="47" spans="1:17">
       <c r="A47" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -6780,7 +6781,7 @@
         <v>3.6</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I55" s="8">
         <v>3.6</v>
@@ -6826,7 +6827,7 @@
         <v>2.6</v>
       </c>
       <c r="Q60" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -6861,7 +6862,7 @@
         <v>1.8</v>
       </c>
       <c r="P64" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -6912,7 +6913,7 @@
         <v>0.6</v>
       </c>
       <c r="P70" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -6931,7 +6932,7 @@
         <v>0.2</v>
       </c>
       <c r="Q72" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:17">
@@ -6939,7 +6940,7 @@
         <v>0</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I73" s="8">
         <v>0</v>
@@ -6963,7 +6964,7 @@
     </row>
     <row r="146" spans="16:16">
       <c r="P146" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>